<commit_message>
Migração de dados - Clientes
Criação do notebook para migração da tabela Clientes
</commit_message>
<xml_diff>
--- a/MIGRAÇÃO PADRÕES NOVO.xlsx
+++ b/MIGRAÇÃO PADRÕES NOVO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haustin.vieira\Downloads\Teste Prático\Advbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\teste-ADVBOX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2233A76F-2813-40B2-A978-A94B47D5652B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FDDE4E-4D7F-48B2-BFD3-FA5CC2BEC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="novo padrão " sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -381,6 +381,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -724,80 +730,80 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
     </row>
-    <row r="3" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:29" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="4" t="s">
+      <c r="N3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
+      <c r="S3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
     </row>
     <row r="4" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -865,56 +871,56 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
     </row>
-    <row r="6" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:29" s="12" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4" t="s">
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4" t="s">
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
     </row>
     <row r="7" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>

</xml_diff>